<commit_message>
1st. Release read from XLSX file "universityInfo.xlsx" two separate sheets "Студенты/Университеты" (by two methods getStudentData() & getUniversityData()), wrote fetched cells to List/Collection & print both Lists to console.
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\IdeaProjects\SFModule29HomeProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D517B3F6-4CCB-4851-AB85-8F38C5BDA72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8468C4E3-ACB2-4A94-B64A-2EF243FA6C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="90" windowWidth="14400" windowHeight="8950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -199,11 +199,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -544,11 +546,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -728,15 +733,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -748,7 +753,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -766,7 +771,7 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2">
@@ -783,7 +788,7 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D3">
@@ -800,7 +805,7 @@
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D4">
@@ -817,7 +822,7 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D5">
@@ -834,7 +839,7 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D6">
@@ -851,7 +856,7 @@
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D7">
@@ -868,7 +873,7 @@
       <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D8">
@@ -880,7 +885,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>